<commit_message>
update search and upload
</commit_message>
<xml_diff>
--- a/Level_1/Search_function/searchdata.xlsx
+++ b/Level_1/Search_function/searchdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Documents_Son\CODING\Software_Testing\Search_function\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Documents_Son\CODING\Software_Testing\Level_1\Search_function\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4FD31D-D4F5-4C88-8C2E-F146D8053443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD22281E-3C04-456F-A9D4-0DC7F6958571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B693AD74-89BF-4A63-9D6D-10EB4586A90B}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>